<commit_message>
Namespace refactoring, groundwork for combat
</commit_message>
<xml_diff>
--- a/Assets/Concepts.xlsx
+++ b/Assets/Concepts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\RogueFrame\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Unity\RogueFrame\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5F9C4E-4FE3-4E6B-9884-5E8C17482B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CE41A6-16BA-492E-AEFF-2AC18C76018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{7ED625D7-40B9-410C-853D-304290349304}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{7ED625D7-40B9-410C-853D-304290349304}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Items" sheetId="5" r:id="rId5"/>
     <sheet name="Mods" sheetId="6" r:id="rId6"/>
     <sheet name="Damage Types" sheetId="7" r:id="rId7"/>
+    <sheet name="Status Effects" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -115,18 +116,12 @@
     <t>Sniper</t>
   </si>
   <si>
-    <t>Nearby burning enemies give strength and hp regeneration</t>
-  </si>
-  <si>
     <t>Ignite an enemy</t>
   </si>
   <si>
     <t>Ult</t>
   </si>
   <si>
-    <t>Flamethrower</t>
-  </si>
-  <si>
     <t>Detonate</t>
   </si>
   <si>
@@ -139,9 +134,6 @@
     <t>Energy?</t>
   </si>
   <si>
-    <t>Chills nearby area</t>
-  </si>
-  <si>
     <t>Map-wide slow, enhances all abilities</t>
   </si>
   <si>
@@ -160,18 +152,12 @@
     <t>Barrier</t>
   </si>
   <si>
-    <t>Heat for weapons or mobility</t>
-  </si>
-  <si>
     <t>Trap an enemy</t>
   </si>
   <si>
     <t>Radial slow</t>
   </si>
   <si>
-    <t>Nature</t>
-  </si>
-  <si>
     <t>Fortress</t>
   </si>
   <si>
@@ -187,15 +173,9 @@
     <t>Grass prevents status</t>
   </si>
   <si>
-    <t>Wings</t>
-  </si>
-  <si>
     <t>Summon natural allies</t>
   </si>
   <si>
-    <t>Enemies less accurate</t>
-  </si>
-  <si>
     <t>Immune to knockback, innate taunt</t>
   </si>
   <si>
@@ -337,9 +317,6 @@
     <t>Modifiers</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Physical</t>
   </si>
   <si>
@@ -397,7 +374,160 @@
     <t>Turret overclocked, gain personal drones</t>
   </si>
   <si>
-    <t>Exalted Claws/Axe?</t>
+    <t>Bleed</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>Stun</t>
+  </si>
+  <si>
+    <t>Miniboss</t>
+  </si>
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>Skrub</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Bludgeon</t>
+  </si>
+  <si>
+    <t>DoT</t>
+  </si>
+  <si>
+    <t>Silence</t>
+  </si>
+  <si>
+    <t>Freeze</t>
+  </si>
+  <si>
+    <t>AoE</t>
+  </si>
+  <si>
+    <t>AoE &amp; Stun</t>
+  </si>
+  <si>
+    <t>Slow all</t>
+  </si>
+  <si>
+    <t>Slow movement</t>
+  </si>
+  <si>
+    <t>Moderate slow movement</t>
+  </si>
+  <si>
+    <t>Big slow movement</t>
+  </si>
+  <si>
+    <t>Reduced accuracy</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Abilities disabled</t>
+  </si>
+  <si>
+    <t>Longer cooldowns</t>
+  </si>
+  <si>
+    <t>Longer cooldowns &amp; slower energy regen</t>
+  </si>
+  <si>
+    <t>Active friendly fire</t>
+  </si>
+  <si>
+    <t>Incidental friendly fire</t>
+  </si>
+  <si>
+    <t>Reduced Incidental friendly fire</t>
+  </si>
+  <si>
+    <t>Heat patch / teleport</t>
+  </si>
+  <si>
+    <t>Blinded</t>
+  </si>
+  <si>
+    <t>Aimlessly flail</t>
+  </si>
+  <si>
+    <t>Reduced cone of vision</t>
+  </si>
+  <si>
+    <t>Reduce saturation and remove outlines</t>
+  </si>
+  <si>
+    <t>Flashbang</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Reduced gravity (&amp; 3d control?)</t>
+  </si>
+  <si>
+    <t>Air blast</t>
+  </si>
+  <si>
+    <t>Hurricane (slow, DoT, armour strip?)</t>
+  </si>
+  <si>
+    <t>Self propulsion</t>
+  </si>
+  <si>
+    <t>Tornados</t>
+  </si>
+  <si>
+    <t>Wind wall</t>
+  </si>
+  <si>
+    <t>Convert incoming damage to AoE heal</t>
+  </si>
+  <si>
+    <t>Hurt self, and spread damage in AoE</t>
+  </si>
+  <si>
+    <t>Damage link</t>
+  </si>
+  <si>
+    <t>Bleed self for AoE buff</t>
+  </si>
+  <si>
+    <t>Nature/Fey</t>
+  </si>
+  <si>
+    <t>Taking damage increases damage output</t>
+  </si>
+  <si>
+    <t>Nearby burning enemies give strength and hp regeneration, all attacks cause fire</t>
+  </si>
+  <si>
+    <t>Chills nearby area, all attacks cause cold</t>
+  </si>
+  <si>
+    <t>Wings allow glide</t>
+  </si>
+  <si>
+    <t>AoE buff (damage resistance?)</t>
+  </si>
+  <si>
+    <t>Masochist / Sadist</t>
+  </si>
+  <si>
+    <t>Melee mega buffed</t>
+  </si>
+  <si>
+    <t>Big health pool increase, abilities buffed, drain (and heal from) nearby enemies</t>
   </si>
 </sst>
 </file>
@@ -433,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -443,6 +573,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,25 +891,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395CF6FB-D269-43B3-BE3D-7EF6E3FE5819}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.07421875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.3046875" customWidth="1"/>
+    <col min="5" max="5" width="10.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -796,7 +929,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -805,36 +938,36 @@
         <v>12</v>
       </c>
       <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>155</v>
       </c>
       <c r="I2" s="2">
         <v>1.1000000000000001</v>
@@ -849,27 +982,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
+        <v>156</v>
       </c>
       <c r="I3" s="2">
         <v>0.8</v>
@@ -884,27 +1017,27 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="50.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="I4" s="2">
         <v>1.2</v>
@@ -919,27 +1052,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I5" s="2">
         <v>0.7</v>
@@ -954,24 +1087,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="H6" s="1" t="str">
         <f>"+Damage and resistance per kill, chance to get back up?"</f>
@@ -990,27 +1123,27 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
@@ -1025,27 +1158,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I8" s="2">
         <v>1.3</v>
@@ -1060,27 +1193,27 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I9" s="2">
         <v>1</v>
@@ -1095,27 +1228,27 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I10" s="2">
         <v>1.2</v>
@@ -1130,27 +1263,27 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I11" s="2">
         <v>1.6</v>
@@ -1165,27 +1298,27 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I12" s="2">
         <v>1.1000000000000001</v>
@@ -1200,27 +1333,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B13" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="I13" s="2">
         <v>0.8</v>
@@ -1233,6 +1366,76 @@
       </c>
       <c r="L13" s="2">
         <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="B14" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>40</v>
+      </c>
+      <c r="K14" s="2">
+        <v>40</v>
+      </c>
+      <c r="L14" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="B15" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>150</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1248,9 +1451,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1276,44 +1479,44 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1329,9 +1532,9 @@
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1370,9 +1573,9 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1402,9 +1605,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1431,9 +1634,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1454,15 +1657,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774D3B7D-C181-418A-841D-C955AA38F338}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1470,30 +1673,237 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB32EE5-9A7B-47A3-9349-448B06101EB1}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.3046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stat Sync & Fixed superfluous error messages
</commit_message>
<xml_diff>
--- a/Assets/Concepts.xlsx
+++ b/Assets/Concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\Unity\RogueFrame\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\RogueFrame\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CE41A6-16BA-492E-AEFF-2AC18C76018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F68ACFD-14F1-4810-BBB4-A7265B2FBFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{7ED625D7-40B9-410C-853D-304290349304}"/>
+    <workbookView xWindow="-28920" yWindow="2460" windowWidth="29040" windowHeight="15840" xr2:uid="{7ED625D7-40B9-410C-853D-304290349304}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -311,9 +311,6 @@
     <t>Crush</t>
   </si>
   <si>
-    <t>Receives less kinetic damage</t>
-  </si>
-  <si>
     <t>Modifiers</t>
   </si>
   <si>
@@ -509,9 +506,6 @@
     <t>Taking damage increases damage output</t>
   </si>
   <si>
-    <t>Nearby burning enemies give strength and hp regeneration, all attacks cause fire</t>
-  </si>
-  <si>
     <t>Chills nearby area, all attacks cause cold</t>
   </si>
   <si>
@@ -528,6 +522,9 @@
   </si>
   <si>
     <t>Big health pool increase, abilities buffed, drain (and heal from) nearby enemies</t>
+  </si>
+  <si>
+    <t>Nearby burning enemies give strength and hp regeneration</t>
   </si>
 </sst>
 </file>
@@ -891,25 +888,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395CF6FB-D269-43B3-BE3D-7EF6E3FE5819}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.3046875" customWidth="1"/>
-    <col min="5" max="5" width="10.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.23046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -947,7 +944,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
@@ -955,19 +952,19 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I2" s="2">
         <v>1.1000000000000001</v>
@@ -982,7 +979,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1002,7 +999,7 @@
         <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I3" s="2">
         <v>0.8</v>
@@ -1017,9 +1014,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="50.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="50.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>41</v>
@@ -1028,16 +1025,16 @@
         <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I4" s="2">
         <v>1.2</v>
@@ -1052,7 +1049,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1087,7 +1084,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1104,7 +1101,7 @@
         <v>34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H6" s="1" t="str">
         <f>"+Damage and resistance per kill, chance to get back up?"</f>
@@ -1123,7 +1120,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>67</v>
       </c>
@@ -1158,7 +1155,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>54</v>
       </c>
@@ -1193,7 +1190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>57</v>
       </c>
@@ -1204,7 +1201,7 @@
         <v>60</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>62</v>
@@ -1228,7 +1225,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>77</v>
       </c>
@@ -1263,7 +1260,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>63</v>
       </c>
@@ -1298,7 +1295,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>83</v>
       </c>
@@ -1317,9 +1314,7 @@
       <c r="G12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1333,27 +1328,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I13" s="2">
         <v>0.8</v>
@@ -1368,27 +1363,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="I14" s="2">
         <v>1.3</v>
@@ -1403,27 +1398,27 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
@@ -1436,6 +1431,14 @@
       </c>
       <c r="L15" s="2">
         <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I16" s="2">
+        <v>50</v>
+      </c>
+      <c r="J16" s="2">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1451,9 +1454,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1479,44 +1482,44 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1532,9 +1535,9 @@
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1573,9 +1576,9 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1605,9 +1608,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1634,9 +1637,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1663,9 +1666,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1673,27 +1676,27 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1706,204 +1709,204 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>116</v>
       </c>
-      <c r="C1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
         <v>121</v>
       </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" t="s">
         <v>125</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>119</v>
       </c>
-      <c r="C5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>128</v>
       </c>
-      <c r="D9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
         <v>132</v>
       </c>
-      <c r="D10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>133</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>134</v>
       </c>
-      <c r="D11" t="s">
-        <v>135</v>
-      </c>
       <c r="E11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
         <v>137</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>138</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" t="s">
         <v>139</v>
-      </c>
-      <c r="D12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>